<commit_message>
Added abstract_forms_data and data FORMS
</commit_message>
<xml_diff>
--- a/design/business_data/preprocessing/initial_data.xlsx
+++ b/design/business_data/preprocessing/initial_data.xlsx
@@ -6,7 +6,6 @@
     <sheet state="visible" name="岗位" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="会员" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="服务类别" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Global" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>岗位名称</t>
   </si>
@@ -64,7 +63,7 @@
     <t>钻石卡</t>
   </si>
   <si>
-    <t>服务类别名称</t>
+    <t>值</t>
   </si>
   <si>
     <t>光电类</t>
@@ -83,12 +82,6 @@
   </si>
   <si>
     <t>注射填充类</t>
-  </si>
-  <si>
-    <t>ORGANIZATION</t>
-  </si>
-  <si>
-    <t>广州颜青医疗美容诊所</t>
   </si>
 </sst>
 </file>
@@ -205,10 +198,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
@@ -724,31 +713,4 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="13.5"/>
-    <col customWidth="1" min="2" max="2" width="17.63"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>